<commit_message>
Runs, added the new column names
</commit_message>
<xml_diff>
--- a/Data/Rustripsdata.xlsx
+++ b/Data/Rustripsdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t xml:space="preserve">Rustrip name</t>
   </si>
@@ -220,100 +220,115 @@
     <t>Christie</t>
   </si>
   <si>
-    <t xml:space="preserve">KABS name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Study line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Eksport og Teknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Kemi- og Bioteknik samt D. Kemiteknik og International Business</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Byggeteknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Process og Innovation, Produktion, Transport og Mobilitet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Vand, bioressourcer og miljømanagement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Softwareteknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. General Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Maskinteknik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Elektroteknologi samt C. Cyberteknologi</t>
-  </si>
-  <si>
-    <t>Ida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Bæredygtigt Energidesign</t>
-  </si>
-  <si>
-    <t>Koch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Byggeri og Infrastruktur &amp; D. Arktisk Byggeri og Infrastruktur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Fødevaresikkerhed og -kvalitet samt D. Fiskeriteknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Medicin og Teknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Life Science og Teknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Geofysik og Rumteknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Design og Innovation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Bygningsdesign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Kemi &amp; Teknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Kunstig Intelligens og Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Sundhedsteknologi samt D. IT-elektronik (SUIT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. IT og Økonomi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Bygningsdesign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Produktion og Konstruktion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D. Elektroteknologi samt D. Elektrisk Energiteknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Fysik og Nanoteknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Data Science og Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Softwareteknologi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C. Matematik og Teknologi</t>
+    <t xml:space="preserve">KABS on the trip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rustrip Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josefine Wibom</t>
+  </si>
+  <si>
+    <t>Campus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emilie Rønbøg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gustav Heron Melhus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 day Danish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anders Strøbæk,Theis Harbers Rix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marika Norby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sophie Plougmand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oliver Sellberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 day mix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thor Deibert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anna Hjort Danielsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niels Boelt Mortensen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August Johannsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eske Haack,Laurits Jürs Hahn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnus Hilarious Ohlin Jepsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lachlan Houston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anna Weilsby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liam Barbosa,Benedicte Jensen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frederik Jørgensen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helene Moesgaard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sarah Ranzow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johan Rosenkrands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tobias Bæk,Marilouise J. Arbøl Tofte</t>
+  </si>
+  <si>
+    <t>Oneday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hannah Leah Herlev Hvid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 day Danish sober</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joakim Vestergaard Rasmussen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mads Kofod Egestad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ea Quie Landgreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas Nielsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benedicte Jensen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malou Liv Enevoldsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonas Bennich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 day mix sober</t>
   </si>
 </sst>
 </file>
@@ -322,14 +337,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
       <color theme="1"/>
-      <sz val="11.000000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -352,11 +367,16 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1499,7 +1519,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1512,267 +1532,451 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.57421875"/>
+  </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" t="s">
+      <c r="C8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="3">
+        <v>9</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="3">
+        <v>8</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="3">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="3">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="3">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="3">
+        <v>8</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="3">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="3">
+        <v>9</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="3">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" ht="14.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="A11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25">
-      <c r="A22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="A26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="A27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="28" ht="14.25">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>97</v>
+      <c r="A28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="3">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>76</v>
+      <c r="A29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="3">
+        <v>13</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>85</v>
+      <c r="A30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="3">
+        <v>13</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>98</v>
+      <c r="A31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="3">
+        <v>7</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="B32" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>